<commit_message>
added the extra ov times
</commit_message>
<xml_diff>
--- a/Data_files/Part_2/Rotterdam_ov_times.xlsx
+++ b/Data_files/Part_2/Rotterdam_ov_times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF96EA2E-E67F-43AF-85C8-F32EC54864C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2591FEF2-8DE0-40DC-AA39-1650738ABE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,7 +464,7 @@
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="F2" sqref="F2:Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,7 +566,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="4">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>25</v>
@@ -575,7 +575,7 @@
         <v>25</v>
       </c>
       <c r="J2" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>25</v>
@@ -590,13 +590,13 @@
         <v>25</v>
       </c>
       <c r="O2" s="4">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="Q2" s="4">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>25</v>
@@ -605,10 +605,10 @@
         <v>25</v>
       </c>
       <c r="T2" s="4">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="U2" s="4">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>25</v>
@@ -640,7 +640,7 @@
         <v>620.44267049999996</v>
       </c>
       <c r="F3" s="3">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>25</v>
@@ -649,7 +649,7 @@
         <v>25</v>
       </c>
       <c r="I3" s="4">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>25</v>
@@ -682,10 +682,10 @@
         <v>25</v>
       </c>
       <c r="T3" s="4">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="U3" s="4">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="V3" s="4" t="s">
         <v>25</v>
@@ -729,7 +729,7 @@
         <v>25</v>
       </c>
       <c r="J4" s="4">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>25</v>
@@ -738,7 +738,7 @@
         <v>25</v>
       </c>
       <c r="M4" s="4">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>25</v>
@@ -797,7 +797,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="4">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>25</v>
@@ -839,7 +839,7 @@
         <v>25</v>
       </c>
       <c r="U5" s="4">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="V5" s="4" t="s">
         <v>25</v>
@@ -848,7 +848,7 @@
         <v>25</v>
       </c>
       <c r="X5" s="4">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Y5" s="4" t="s">
         <v>25</v>
@@ -871,13 +871,13 @@
         <v>45.405584189999999</v>
       </c>
       <c r="F6" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H6" s="4">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>25</v>
@@ -886,25 +886,25 @@
         <v>25</v>
       </c>
       <c r="K6" s="4">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="L6" s="4">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="M6" s="4">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="N6" s="4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O6" s="4">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="P6" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Q6" s="4">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>25</v>
@@ -916,7 +916,7 @@
         <v>25</v>
       </c>
       <c r="U6" s="4">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="V6" s="4" t="s">
         <v>25</v>
@@ -925,10 +925,10 @@
         <v>25</v>
       </c>
       <c r="X6" s="4">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="Y6" s="4">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
@@ -960,7 +960,7 @@
         <v>25</v>
       </c>
       <c r="J7" s="4">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>25</v>
@@ -975,13 +975,13 @@
         <v>25</v>
       </c>
       <c r="O7" s="4">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="Q7" s="4">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>25</v>
@@ -1037,7 +1037,7 @@
         <v>25</v>
       </c>
       <c r="J8" s="4">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>25</v>
@@ -1046,37 +1046,37 @@
         <v>25</v>
       </c>
       <c r="M8" s="4">
+        <v>15</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R8" s="4">
+        <v>27</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="V8" s="4">
         <v>14</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R8" s="4">
-        <v>30</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="V8" s="4">
-        <v>22</v>
-      </c>
       <c r="W8" s="4">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>25</v>
@@ -1108,19 +1108,19 @@
         <v>25</v>
       </c>
       <c r="H9" s="4">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="J9" s="4">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L9" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>25</v>
@@ -1138,7 +1138,7 @@
         <v>25</v>
       </c>
       <c r="R9" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>25</v>
@@ -1150,10 +1150,10 @@
         <v>25</v>
       </c>
       <c r="V9" s="4">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="W9" s="4">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="X9" s="4" t="s">
         <v>25</v>
@@ -1191,7 +1191,7 @@
         <v>25</v>
       </c>
       <c r="J10" s="4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>25</v>
@@ -1233,7 +1233,7 @@
         <v>25</v>
       </c>
       <c r="X10" s="4">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="Y10" s="4" t="s">
         <v>25</v>
@@ -1256,7 +1256,7 @@
         <v>21.765798969999999</v>
       </c>
       <c r="F11" s="4">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>25</v>
@@ -1268,10 +1268,10 @@
         <v>25</v>
       </c>
       <c r="J11" s="4">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="K11" s="4">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>25</v>
@@ -1345,7 +1345,7 @@
         <v>25</v>
       </c>
       <c r="J12" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>25</v>
@@ -1387,10 +1387,10 @@
         <v>25</v>
       </c>
       <c r="X12" s="4">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="Y12" s="4">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
@@ -1410,7 +1410,7 @@
         <v>85.981795599999998</v>
       </c>
       <c r="F13" s="4">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>25</v>
@@ -1422,10 +1422,10 @@
         <v>25</v>
       </c>
       <c r="J13" s="4">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="K13" s="4">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>25</v>
@@ -1446,13 +1446,13 @@
         <v>25</v>
       </c>
       <c r="R13" s="4">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="S13" s="4">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="T13" s="4">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>25</v>
@@ -1505,10 +1505,10 @@
         <v>25</v>
       </c>
       <c r="L14" s="4">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M14" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>25</v>
@@ -1520,7 +1520,7 @@
         <v>25</v>
       </c>
       <c r="Q14" s="4">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="R14" s="3" t="s">
         <v>25</v>
@@ -1535,10 +1535,10 @@
         <v>25</v>
       </c>
       <c r="V14" s="4">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="W14" s="4">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="X14" s="4" t="s">
         <v>25</v>
@@ -1597,7 +1597,7 @@
         <v>25</v>
       </c>
       <c r="Q15" s="4">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>25</v>
@@ -1641,10 +1641,10 @@
         <v>126.6450923</v>
       </c>
       <c r="F16" s="4">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G16" s="4">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>25</v>
@@ -1674,7 +1674,7 @@
         <v>25</v>
       </c>
       <c r="Q16" s="4">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>25</v>
@@ -1718,19 +1718,19 @@
         <v>139.99559070000001</v>
       </c>
       <c r="F17" s="4">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="G17" s="4">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>25</v>
       </c>
       <c r="I17" s="4">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="J17" s="4">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>25</v>
@@ -1775,7 +1775,7 @@
         <v>25</v>
       </c>
       <c r="Y17" s="4">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
@@ -1813,10 +1813,10 @@
         <v>25</v>
       </c>
       <c r="L18" s="4">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="M18" s="4">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>25</v>
@@ -1831,7 +1831,7 @@
         <v>25</v>
       </c>
       <c r="R18" s="4">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="S18" s="4" t="s">
         <v>25</v>
@@ -1846,7 +1846,7 @@
         <v>25</v>
       </c>
       <c r="W18" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="X18" s="4" t="s">
         <v>25</v>
@@ -1890,10 +1890,10 @@
         <v>25</v>
       </c>
       <c r="L19" s="4">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M19" s="4">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>25</v>
@@ -1908,7 +1908,7 @@
         <v>25</v>
       </c>
       <c r="R19" s="4">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="S19" s="4" t="s">
         <v>25</v>
@@ -1920,13 +1920,13 @@
         <v>25</v>
       </c>
       <c r="V19" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="W19" s="3" t="s">
         <v>25</v>
       </c>
       <c r="X19" s="4">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="Y19" s="4" t="s">
         <v>25</v>
@@ -1958,10 +1958,10 @@
         <v>25</v>
       </c>
       <c r="I20" s="4">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J20" s="4">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>25</v>
@@ -1973,13 +1973,13 @@
         <v>25</v>
       </c>
       <c r="N20" s="4">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O20" s="4" t="s">
         <v>25</v>
       </c>
       <c r="P20" s="4">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="Q20" s="4" t="s">
         <v>25</v>
@@ -2000,13 +2000,13 @@
         <v>25</v>
       </c>
       <c r="W20" s="4">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="Y20" s="4">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
@@ -2038,7 +2038,7 @@
         <v>25</v>
       </c>
       <c r="J21" s="4">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>25</v>
@@ -2056,7 +2056,7 @@
         <v>25</v>
       </c>
       <c r="P21" s="4">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="Q21" s="4" t="s">
         <v>25</v>
@@ -2071,7 +2071,7 @@
         <v>25</v>
       </c>
       <c r="U21" s="4">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="V21" s="4" t="s">
         <v>25</v>
@@ -2080,7 +2080,7 @@
         <v>25</v>
       </c>
       <c r="X21" s="4">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="Y21" s="3" t="s">
         <v>25</v>

</xml_diff>